<commit_message>
📅 Monthly schedule for 09/2025
</commit_message>
<xml_diff>
--- a/schedules/schedule_09_2025.xlsx
+++ b/schedules/schedule_09_2025.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="187">
   <si>
     <t>September 2025</t>
   </si>
@@ -54,10 +54,7 @@
     <t>3PM-5PM</t>
   </si>
   <si>
-    <t>R CC</t>
-  </si>
-  <si>
-    <t>bb bb</t>
+    <t>New A</t>
   </si>
   <si>
     <t>Name</t>
@@ -144,16 +141,16 @@
     <t>2025-09-30</t>
   </si>
   <si>
-    <t>R CC, bb bb</t>
-  </si>
-  <si>
     <t>Warnings</t>
   </si>
   <si>
     <t>Warning</t>
   </si>
   <si>
-    <t>Only 2 for 2025-09-01 9AM-11AM</t>
+    <t>No senior for 2025-09-01 9AM-11AM</t>
+  </si>
+  <si>
+    <t>Only 0 for 2025-09-01 9AM-11AM</t>
   </si>
   <si>
     <t>No senior for 2025-09-01 11AM-1PM</t>
@@ -171,22 +168,25 @@
     <t>No senior for 2025-09-01 3PM-5PM</t>
   </si>
   <si>
-    <t>Only 1 for 2025-09-01 3PM-5PM</t>
-  </si>
-  <si>
-    <t>Only 1 for 2025-09-02 9AM-11AM</t>
+    <t>Only 0 for 2025-09-01 3PM-5PM</t>
+  </si>
+  <si>
+    <t>No senior for 2025-09-02 9AM-11AM</t>
+  </si>
+  <si>
+    <t>Only 0 for 2025-09-02 9AM-11AM</t>
   </si>
   <si>
     <t>No senior for 2025-09-02 11AM-1PM</t>
   </si>
   <si>
-    <t>Only 1 for 2025-09-02 11AM-1PM</t>
+    <t>Only 0 for 2025-09-02 11AM-1PM</t>
   </si>
   <si>
     <t>No senior for 2025-09-02 1PM-3PM</t>
   </si>
   <si>
-    <t>Only 1 for 2025-09-02 1PM-3PM</t>
+    <t>Only 0 for 2025-09-02 1PM-3PM</t>
   </si>
   <si>
     <t>No senior for 2025-09-02 3PM-5PM</t>
@@ -198,46 +198,31 @@
     <t>Only 1 for 2025-09-03 9AM-11AM</t>
   </si>
   <si>
-    <t>No senior for 2025-09-03 11AM-1PM</t>
-  </si>
-  <si>
     <t>Only 1 for 2025-09-03 11AM-1PM</t>
   </si>
   <si>
-    <t>No senior for 2025-09-03 1PM-3PM</t>
-  </si>
-  <si>
     <t>Only 1 for 2025-09-03 1PM-3PM</t>
   </si>
   <si>
-    <t>No senior for 2025-09-03 3PM-5PM</t>
-  </si>
-  <si>
-    <t>Only 0 for 2025-09-03 3PM-5PM</t>
-  </si>
-  <si>
-    <t>Only 2 for 2025-09-04 9AM-11AM</t>
-  </si>
-  <si>
-    <t>No senior for 2025-09-04 11AM-1PM</t>
-  </si>
-  <si>
-    <t>Only 0 for 2025-09-04 11AM-1PM</t>
-  </si>
-  <si>
-    <t>No senior for 2025-09-04 1PM-3PM</t>
-  </si>
-  <si>
-    <t>Only 0 for 2025-09-04 1PM-3PM</t>
-  </si>
-  <si>
-    <t>No senior for 2025-09-04 3PM-5PM</t>
+    <t>Only 1 for 2025-09-03 3PM-5PM</t>
+  </si>
+  <si>
+    <t>Only 1 for 2025-09-04 9AM-11AM</t>
+  </si>
+  <si>
+    <t>Only 1 for 2025-09-04 11AM-1PM</t>
+  </si>
+  <si>
+    <t>Only 1 for 2025-09-04 1PM-3PM</t>
   </si>
   <si>
     <t>Only 1 for 2025-09-04 3PM-5PM</t>
   </si>
   <si>
-    <t>Only 1 for 2025-09-05 9AM-11AM</t>
+    <t>No senior for 2025-09-05 9AM-11AM</t>
+  </si>
+  <si>
+    <t>Only 0 for 2025-09-05 9AM-11AM</t>
   </si>
   <si>
     <t>No senior for 2025-09-05 11AM-1PM</t>
@@ -258,7 +243,10 @@
     <t>Only 0 for 2025-09-05 3PM-5PM</t>
   </si>
   <si>
-    <t>Only 2 for 2025-09-08 9AM-11AM</t>
+    <t>No senior for 2025-09-08 9AM-11AM</t>
+  </si>
+  <si>
+    <t>Only 0 for 2025-09-08 9AM-11AM</t>
   </si>
   <si>
     <t>No senior for 2025-09-08 11AM-1PM</t>
@@ -276,22 +264,25 @@
     <t>No senior for 2025-09-08 3PM-5PM</t>
   </si>
   <si>
-    <t>Only 1 for 2025-09-08 3PM-5PM</t>
-  </si>
-  <si>
-    <t>Only 1 for 2025-09-09 9AM-11AM</t>
+    <t>Only 0 for 2025-09-08 3PM-5PM</t>
+  </si>
+  <si>
+    <t>No senior for 2025-09-09 9AM-11AM</t>
+  </si>
+  <si>
+    <t>Only 0 for 2025-09-09 9AM-11AM</t>
   </si>
   <si>
     <t>No senior for 2025-09-09 11AM-1PM</t>
   </si>
   <si>
-    <t>Only 1 for 2025-09-09 11AM-1PM</t>
+    <t>Only 0 for 2025-09-09 11AM-1PM</t>
   </si>
   <si>
     <t>No senior for 2025-09-09 1PM-3PM</t>
   </si>
   <si>
-    <t>Only 1 for 2025-09-09 1PM-3PM</t>
+    <t>Only 0 for 2025-09-09 1PM-3PM</t>
   </si>
   <si>
     <t>No senior for 2025-09-09 3PM-5PM</t>
@@ -303,46 +294,31 @@
     <t>Only 1 for 2025-09-10 9AM-11AM</t>
   </si>
   <si>
-    <t>No senior for 2025-09-10 11AM-1PM</t>
-  </si>
-  <si>
     <t>Only 1 for 2025-09-10 11AM-1PM</t>
   </si>
   <si>
-    <t>No senior for 2025-09-10 1PM-3PM</t>
-  </si>
-  <si>
     <t>Only 1 for 2025-09-10 1PM-3PM</t>
   </si>
   <si>
-    <t>No senior for 2025-09-10 3PM-5PM</t>
-  </si>
-  <si>
-    <t>Only 0 for 2025-09-10 3PM-5PM</t>
-  </si>
-  <si>
-    <t>Only 2 for 2025-09-11 9AM-11AM</t>
-  </si>
-  <si>
-    <t>No senior for 2025-09-11 11AM-1PM</t>
-  </si>
-  <si>
-    <t>Only 0 for 2025-09-11 11AM-1PM</t>
-  </si>
-  <si>
-    <t>No senior for 2025-09-11 1PM-3PM</t>
-  </si>
-  <si>
-    <t>Only 0 for 2025-09-11 1PM-3PM</t>
-  </si>
-  <si>
-    <t>No senior for 2025-09-11 3PM-5PM</t>
+    <t>Only 1 for 2025-09-10 3PM-5PM</t>
+  </si>
+  <si>
+    <t>Only 1 for 2025-09-11 9AM-11AM</t>
+  </si>
+  <si>
+    <t>Only 1 for 2025-09-11 11AM-1PM</t>
+  </si>
+  <si>
+    <t>Only 1 for 2025-09-11 1PM-3PM</t>
   </si>
   <si>
     <t>Only 1 for 2025-09-11 3PM-5PM</t>
   </si>
   <si>
-    <t>Only 1 for 2025-09-12 9AM-11AM</t>
+    <t>No senior for 2025-09-12 9AM-11AM</t>
+  </si>
+  <si>
+    <t>Only 0 for 2025-09-12 9AM-11AM</t>
   </si>
   <si>
     <t>No senior for 2025-09-12 11AM-1PM</t>
@@ -363,7 +339,10 @@
     <t>Only 0 for 2025-09-12 3PM-5PM</t>
   </si>
   <si>
-    <t>Only 2 for 2025-09-15 9AM-11AM</t>
+    <t>No senior for 2025-09-15 9AM-11AM</t>
+  </si>
+  <si>
+    <t>Only 0 for 2025-09-15 9AM-11AM</t>
   </si>
   <si>
     <t>No senior for 2025-09-15 11AM-1PM</t>
@@ -381,22 +360,25 @@
     <t>No senior for 2025-09-15 3PM-5PM</t>
   </si>
   <si>
-    <t>Only 1 for 2025-09-15 3PM-5PM</t>
-  </si>
-  <si>
-    <t>Only 1 for 2025-09-16 9AM-11AM</t>
+    <t>Only 0 for 2025-09-15 3PM-5PM</t>
+  </si>
+  <si>
+    <t>No senior for 2025-09-16 9AM-11AM</t>
+  </si>
+  <si>
+    <t>Only 0 for 2025-09-16 9AM-11AM</t>
   </si>
   <si>
     <t>No senior for 2025-09-16 11AM-1PM</t>
   </si>
   <si>
-    <t>Only 1 for 2025-09-16 11AM-1PM</t>
+    <t>Only 0 for 2025-09-16 11AM-1PM</t>
   </si>
   <si>
     <t>No senior for 2025-09-16 1PM-3PM</t>
   </si>
   <si>
-    <t>Only 1 for 2025-09-16 1PM-3PM</t>
+    <t>Only 0 for 2025-09-16 1PM-3PM</t>
   </si>
   <si>
     <t>No senior for 2025-09-16 3PM-5PM</t>
@@ -408,46 +390,31 @@
     <t>Only 1 for 2025-09-17 9AM-11AM</t>
   </si>
   <si>
-    <t>No senior for 2025-09-17 11AM-1PM</t>
-  </si>
-  <si>
     <t>Only 1 for 2025-09-17 11AM-1PM</t>
   </si>
   <si>
-    <t>No senior for 2025-09-17 1PM-3PM</t>
-  </si>
-  <si>
     <t>Only 1 for 2025-09-17 1PM-3PM</t>
   </si>
   <si>
-    <t>No senior for 2025-09-17 3PM-5PM</t>
-  </si>
-  <si>
-    <t>Only 0 for 2025-09-17 3PM-5PM</t>
-  </si>
-  <si>
-    <t>Only 2 for 2025-09-18 9AM-11AM</t>
-  </si>
-  <si>
-    <t>No senior for 2025-09-18 11AM-1PM</t>
-  </si>
-  <si>
-    <t>Only 0 for 2025-09-18 11AM-1PM</t>
-  </si>
-  <si>
-    <t>No senior for 2025-09-18 1PM-3PM</t>
-  </si>
-  <si>
-    <t>Only 0 for 2025-09-18 1PM-3PM</t>
-  </si>
-  <si>
-    <t>No senior for 2025-09-18 3PM-5PM</t>
+    <t>Only 1 for 2025-09-17 3PM-5PM</t>
+  </si>
+  <si>
+    <t>Only 1 for 2025-09-18 9AM-11AM</t>
+  </si>
+  <si>
+    <t>Only 1 for 2025-09-18 11AM-1PM</t>
+  </si>
+  <si>
+    <t>Only 1 for 2025-09-18 1PM-3PM</t>
   </si>
   <si>
     <t>Only 1 for 2025-09-18 3PM-5PM</t>
   </si>
   <si>
-    <t>Only 1 for 2025-09-19 9AM-11AM</t>
+    <t>No senior for 2025-09-19 9AM-11AM</t>
+  </si>
+  <si>
+    <t>Only 0 for 2025-09-19 9AM-11AM</t>
   </si>
   <si>
     <t>No senior for 2025-09-19 11AM-1PM</t>
@@ -468,7 +435,10 @@
     <t>Only 0 for 2025-09-19 3PM-5PM</t>
   </si>
   <si>
-    <t>Only 2 for 2025-09-22 9AM-11AM</t>
+    <t>No senior for 2025-09-22 9AM-11AM</t>
+  </si>
+  <si>
+    <t>Only 0 for 2025-09-22 9AM-11AM</t>
   </si>
   <si>
     <t>No senior for 2025-09-22 11AM-1PM</t>
@@ -486,22 +456,25 @@
     <t>No senior for 2025-09-22 3PM-5PM</t>
   </si>
   <si>
-    <t>Only 1 for 2025-09-22 3PM-5PM</t>
-  </si>
-  <si>
-    <t>Only 1 for 2025-09-23 9AM-11AM</t>
+    <t>Only 0 for 2025-09-22 3PM-5PM</t>
+  </si>
+  <si>
+    <t>No senior for 2025-09-23 9AM-11AM</t>
+  </si>
+  <si>
+    <t>Only 0 for 2025-09-23 9AM-11AM</t>
   </si>
   <si>
     <t>No senior for 2025-09-23 11AM-1PM</t>
   </si>
   <si>
-    <t>Only 1 for 2025-09-23 11AM-1PM</t>
+    <t>Only 0 for 2025-09-23 11AM-1PM</t>
   </si>
   <si>
     <t>No senior for 2025-09-23 1PM-3PM</t>
   </si>
   <si>
-    <t>Only 1 for 2025-09-23 1PM-3PM</t>
+    <t>Only 0 for 2025-09-23 1PM-3PM</t>
   </si>
   <si>
     <t>No senior for 2025-09-23 3PM-5PM</t>
@@ -513,46 +486,31 @@
     <t>Only 1 for 2025-09-24 9AM-11AM</t>
   </si>
   <si>
-    <t>No senior for 2025-09-24 11AM-1PM</t>
-  </si>
-  <si>
     <t>Only 1 for 2025-09-24 11AM-1PM</t>
   </si>
   <si>
-    <t>No senior for 2025-09-24 1PM-3PM</t>
-  </si>
-  <si>
     <t>Only 1 for 2025-09-24 1PM-3PM</t>
   </si>
   <si>
-    <t>No senior for 2025-09-24 3PM-5PM</t>
-  </si>
-  <si>
-    <t>Only 0 for 2025-09-24 3PM-5PM</t>
-  </si>
-  <si>
-    <t>Only 2 for 2025-09-25 9AM-11AM</t>
-  </si>
-  <si>
-    <t>No senior for 2025-09-25 11AM-1PM</t>
-  </si>
-  <si>
-    <t>Only 0 for 2025-09-25 11AM-1PM</t>
-  </si>
-  <si>
-    <t>No senior for 2025-09-25 1PM-3PM</t>
-  </si>
-  <si>
-    <t>Only 0 for 2025-09-25 1PM-3PM</t>
-  </si>
-  <si>
-    <t>No senior for 2025-09-25 3PM-5PM</t>
+    <t>Only 1 for 2025-09-24 3PM-5PM</t>
+  </si>
+  <si>
+    <t>Only 1 for 2025-09-25 9AM-11AM</t>
+  </si>
+  <si>
+    <t>Only 1 for 2025-09-25 11AM-1PM</t>
+  </si>
+  <si>
+    <t>Only 1 for 2025-09-25 1PM-3PM</t>
   </si>
   <si>
     <t>Only 1 for 2025-09-25 3PM-5PM</t>
   </si>
   <si>
-    <t>Only 1 for 2025-09-26 9AM-11AM</t>
+    <t>No senior for 2025-09-26 9AM-11AM</t>
+  </si>
+  <si>
+    <t>Only 0 for 2025-09-26 9AM-11AM</t>
   </si>
   <si>
     <t>No senior for 2025-09-26 11AM-1PM</t>
@@ -573,7 +531,10 @@
     <t>Only 0 for 2025-09-26 3PM-5PM</t>
   </si>
   <si>
-    <t>Only 2 for 2025-09-29 9AM-11AM</t>
+    <t>No senior for 2025-09-29 9AM-11AM</t>
+  </si>
+  <si>
+    <t>Only 0 for 2025-09-29 9AM-11AM</t>
   </si>
   <si>
     <t>No senior for 2025-09-29 11AM-1PM</t>
@@ -591,22 +552,25 @@
     <t>No senior for 2025-09-29 3PM-5PM</t>
   </si>
   <si>
-    <t>Only 1 for 2025-09-29 3PM-5PM</t>
-  </si>
-  <si>
-    <t>Only 1 for 2025-09-30 9AM-11AM</t>
+    <t>Only 0 for 2025-09-29 3PM-5PM</t>
+  </si>
+  <si>
+    <t>No senior for 2025-09-30 9AM-11AM</t>
+  </si>
+  <si>
+    <t>Only 0 for 2025-09-30 9AM-11AM</t>
   </si>
   <si>
     <t>No senior for 2025-09-30 11AM-1PM</t>
   </si>
   <si>
-    <t>Only 1 for 2025-09-30 11AM-1PM</t>
+    <t>Only 0 for 2025-09-30 11AM-1PM</t>
   </si>
   <si>
     <t>No senior for 2025-09-30 1PM-3PM</t>
   </si>
   <si>
-    <t>Only 1 for 2025-09-30 1PM-3PM</t>
+    <t>Only 0 for 2025-09-30 1PM-3PM</t>
   </si>
   <si>
     <t>No senior for 2025-09-30 3PM-5PM</t>
@@ -1141,15 +1105,11 @@
       <c r="B3" s="4">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="C3" s="5"/>
       <c r="D3" s="4">
         <v>2</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="E3" s="5"/>
       <c r="F3" s="4">
         <v>3</v>
       </c>
@@ -1165,9 +1125,7 @@
       <c r="J3" s="4">
         <v>5</v>
       </c>
-      <c r="K3" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="K3" s="5"/>
       <c r="L3" s="4">
         <v>6</v>
       </c>
@@ -1180,17 +1138,13 @@
     <row r="4" spans="1:15">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="C4" s="5"/>
       <c r="D4" s="4"/>
       <c r="E4" s="5"/>
       <c r="F4" s="4"/>
       <c r="G4" s="5"/>
       <c r="H4" s="4"/>
-      <c r="I4" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="I4" s="5"/>
       <c r="J4" s="4"/>
       <c r="K4" s="5"/>
       <c r="L4" s="4"/>
@@ -1222,15 +1176,15 @@
       <c r="B6" s="4"/>
       <c r="C6" s="6"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="E6" s="6"/>
       <c r="F6" s="4"/>
       <c r="G6" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H6" s="4"/>
-      <c r="I6" s="6"/>
+      <c r="I6" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="J6" s="4"/>
       <c r="K6" s="6"/>
       <c r="L6" s="4"/>
@@ -1279,15 +1233,15 @@
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="E9" s="5"/>
       <c r="F9" s="4"/>
       <c r="G9" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H9" s="4"/>
-      <c r="I9" s="5"/>
+      <c r="I9" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="J9" s="4"/>
       <c r="K9" s="5"/>
       <c r="L9" s="4"/>
@@ -1334,16 +1288,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="4"/>
-      <c r="C12" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="C12" s="6"/>
       <c r="D12" s="4"/>
       <c r="E12" s="6"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="6"/>
+      <c r="G12" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="H12" s="4"/>
       <c r="I12" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="6"/>
@@ -1393,15 +1347,11 @@
       <c r="B15" s="4">
         <v>8</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="C15" s="5"/>
       <c r="D15" s="4">
         <v>9</v>
       </c>
-      <c r="E15" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="E15" s="5"/>
       <c r="F15" s="4">
         <v>10</v>
       </c>
@@ -1417,9 +1367,7 @@
       <c r="J15" s="4">
         <v>12</v>
       </c>
-      <c r="K15" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="K15" s="5"/>
       <c r="L15" s="4">
         <v>13</v>
       </c>
@@ -1432,17 +1380,13 @@
     <row r="16" spans="1:15">
       <c r="A16" s="7"/>
       <c r="B16" s="4"/>
-      <c r="C16" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="C16" s="5"/>
       <c r="D16" s="4"/>
       <c r="E16" s="5"/>
       <c r="F16" s="4"/>
       <c r="G16" s="5"/>
       <c r="H16" s="4"/>
-      <c r="I16" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="I16" s="5"/>
       <c r="J16" s="4"/>
       <c r="K16" s="5"/>
       <c r="L16" s="4"/>
@@ -1474,15 +1418,15 @@
       <c r="B18" s="4"/>
       <c r="C18" s="6"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="E18" s="6"/>
       <c r="F18" s="4"/>
       <c r="G18" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H18" s="4"/>
-      <c r="I18" s="6"/>
+      <c r="I18" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="J18" s="4"/>
       <c r="K18" s="6"/>
       <c r="L18" s="4"/>
@@ -1531,15 +1475,15 @@
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="E21" s="5"/>
       <c r="F21" s="4"/>
       <c r="G21" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H21" s="4"/>
-      <c r="I21" s="5"/>
+      <c r="I21" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="J21" s="4"/>
       <c r="K21" s="5"/>
       <c r="L21" s="4"/>
@@ -1586,16 +1530,16 @@
         <v>11</v>
       </c>
       <c r="B24" s="4"/>
-      <c r="C24" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="C24" s="6"/>
       <c r="D24" s="4"/>
       <c r="E24" s="6"/>
       <c r="F24" s="4"/>
-      <c r="G24" s="6"/>
+      <c r="G24" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="H24" s="4"/>
       <c r="I24" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J24" s="4"/>
       <c r="K24" s="6"/>
@@ -1645,15 +1589,11 @@
       <c r="B27" s="4">
         <v>15</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="C27" s="5"/>
       <c r="D27" s="4">
         <v>16</v>
       </c>
-      <c r="E27" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="E27" s="5"/>
       <c r="F27" s="4">
         <v>17</v>
       </c>
@@ -1669,9 +1609,7 @@
       <c r="J27" s="4">
         <v>19</v>
       </c>
-      <c r="K27" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="K27" s="5"/>
       <c r="L27" s="4">
         <v>20</v>
       </c>
@@ -1684,17 +1622,13 @@
     <row r="28" spans="1:15">
       <c r="A28" s="3"/>
       <c r="B28" s="4"/>
-      <c r="C28" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="C28" s="5"/>
       <c r="D28" s="4"/>
       <c r="E28" s="5"/>
       <c r="F28" s="4"/>
       <c r="G28" s="5"/>
       <c r="H28" s="4"/>
-      <c r="I28" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="I28" s="5"/>
       <c r="J28" s="4"/>
       <c r="K28" s="5"/>
       <c r="L28" s="4"/>
@@ -1726,15 +1660,15 @@
       <c r="B30" s="4"/>
       <c r="C30" s="6"/>
       <c r="D30" s="4"/>
-      <c r="E30" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="E30" s="6"/>
       <c r="F30" s="4"/>
       <c r="G30" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H30" s="4"/>
-      <c r="I30" s="6"/>
+      <c r="I30" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="J30" s="4"/>
       <c r="K30" s="6"/>
       <c r="L30" s="4"/>
@@ -1783,15 +1717,15 @@
       <c r="B33" s="4"/>
       <c r="C33" s="5"/>
       <c r="D33" s="4"/>
-      <c r="E33" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="E33" s="5"/>
       <c r="F33" s="4"/>
       <c r="G33" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H33" s="4"/>
-      <c r="I33" s="5"/>
+      <c r="I33" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="J33" s="4"/>
       <c r="K33" s="5"/>
       <c r="L33" s="4"/>
@@ -1838,16 +1772,16 @@
         <v>11</v>
       </c>
       <c r="B36" s="4"/>
-      <c r="C36" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="C36" s="6"/>
       <c r="D36" s="4"/>
       <c r="E36" s="6"/>
       <c r="F36" s="4"/>
-      <c r="G36" s="6"/>
+      <c r="G36" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="H36" s="4"/>
       <c r="I36" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J36" s="4"/>
       <c r="K36" s="6"/>
@@ -1897,15 +1831,11 @@
       <c r="B39" s="4">
         <v>22</v>
       </c>
-      <c r="C39" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="C39" s="5"/>
       <c r="D39" s="4">
         <v>23</v>
       </c>
-      <c r="E39" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="E39" s="5"/>
       <c r="F39" s="4">
         <v>24</v>
       </c>
@@ -1921,9 +1851,7 @@
       <c r="J39" s="4">
         <v>26</v>
       </c>
-      <c r="K39" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="K39" s="5"/>
       <c r="L39" s="4">
         <v>27</v>
       </c>
@@ -1936,17 +1864,13 @@
     <row r="40" spans="1:15">
       <c r="A40" s="7"/>
       <c r="B40" s="4"/>
-      <c r="C40" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="C40" s="5"/>
       <c r="D40" s="4"/>
       <c r="E40" s="5"/>
       <c r="F40" s="4"/>
       <c r="G40" s="5"/>
       <c r="H40" s="4"/>
-      <c r="I40" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="I40" s="5"/>
       <c r="J40" s="4"/>
       <c r="K40" s="5"/>
       <c r="L40" s="4"/>
@@ -1978,15 +1902,15 @@
       <c r="B42" s="4"/>
       <c r="C42" s="6"/>
       <c r="D42" s="4"/>
-      <c r="E42" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="E42" s="6"/>
       <c r="F42" s="4"/>
       <c r="G42" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H42" s="4"/>
-      <c r="I42" s="6"/>
+      <c r="I42" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="J42" s="4"/>
       <c r="K42" s="6"/>
       <c r="L42" s="4"/>
@@ -2035,15 +1959,15 @@
       <c r="B45" s="4"/>
       <c r="C45" s="5"/>
       <c r="D45" s="4"/>
-      <c r="E45" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="E45" s="5"/>
       <c r="F45" s="4"/>
       <c r="G45" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H45" s="4"/>
-      <c r="I45" s="5"/>
+      <c r="I45" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="J45" s="4"/>
       <c r="K45" s="5"/>
       <c r="L45" s="4"/>
@@ -2090,16 +2014,16 @@
         <v>11</v>
       </c>
       <c r="B48" s="4"/>
-      <c r="C48" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="C48" s="6"/>
       <c r="D48" s="4"/>
       <c r="E48" s="6"/>
       <c r="F48" s="4"/>
-      <c r="G48" s="6"/>
+      <c r="G48" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="H48" s="4"/>
       <c r="I48" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J48" s="4"/>
       <c r="K48" s="6"/>
@@ -2149,15 +2073,11 @@
       <c r="B51" s="4">
         <v>29</v>
       </c>
-      <c r="C51" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="C51" s="5"/>
       <c r="D51" s="4">
         <v>30</v>
       </c>
-      <c r="E51" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="E51" s="5"/>
       <c r="F51" s="8"/>
       <c r="G51" s="8"/>
       <c r="H51" s="8"/>
@@ -2172,9 +2092,7 @@
     <row r="52" spans="1:15">
       <c r="A52" s="3"/>
       <c r="B52" s="4"/>
-      <c r="C52" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="C52" s="5"/>
       <c r="D52" s="4"/>
       <c r="E52" s="5"/>
       <c r="F52" s="8"/>
@@ -2212,9 +2130,7 @@
       <c r="B54" s="4"/>
       <c r="C54" s="6"/>
       <c r="D54" s="4"/>
-      <c r="E54" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="E54" s="6"/>
       <c r="F54" s="8"/>
       <c r="G54" s="8"/>
       <c r="H54" s="8"/>
@@ -2267,9 +2183,7 @@
       <c r="B57" s="4"/>
       <c r="C57" s="5"/>
       <c r="D57" s="4"/>
-      <c r="E57" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="E57" s="5"/>
       <c r="F57" s="8"/>
       <c r="G57" s="8"/>
       <c r="H57" s="8"/>
@@ -2320,9 +2234,7 @@
         <v>11</v>
       </c>
       <c r="B60" s="4"/>
-      <c r="C60" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="C60" s="6"/>
       <c r="D60" s="4"/>
       <c r="E60" s="6"/>
       <c r="F60" s="8"/>
@@ -2442,7 +2354,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2454,13 +2366,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>15</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2468,22 +2380,10 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C2" s="10">
-        <f>HYPERLINK("webcal://meghanuni.github.io/smr_scheduler/ics/a665a459.ics", "Subscribe")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3">
-        <v>36</v>
-      </c>
-      <c r="C3" s="10">
-        <f>HYPERLINK("webcal://meghanuni.github.io/smr_scheduler/ics/8d23cf6c.ics", "Subscribe")</f>
+        <f>HYPERLINK("webcal://meghanuni.github.io/smr_scheduler/ics/03ac6742.ics", "Subscribe")</f>
         <v>0</v>
       </c>
     </row>
@@ -2494,7 +2394,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C247"/>
+  <dimension ref="A1:C237"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2505,40 +2405,37 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="11" t="s">
         <v>18</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="C2" s="12" t="s">
         <v>18</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -2546,7 +2443,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -2554,51 +2451,39 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -2606,7 +2491,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
@@ -2617,86 +2502,92 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
       </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
       </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
         <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
       </c>
-      <c r="C19" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
         <v>9</v>
@@ -2704,7 +2595,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
@@ -2712,7 +2603,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
         <v>11</v>
@@ -2720,18 +2611,15 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
       </c>
-      <c r="C23" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
@@ -2739,7 +2627,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>10</v>
@@ -2747,51 +2635,39 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>11</v>
       </c>
-      <c r="C26" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
         <v>8</v>
       </c>
-      <c r="C27" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" t="s">
         <v>9</v>
       </c>
-      <c r="C28" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
       </c>
-      <c r="C29" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B30" t="s">
         <v>11</v>
@@ -2799,7 +2675,7 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B31" t="s">
         <v>8</v>
@@ -2810,86 +2686,92 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B32" t="s">
         <v>9</v>
       </c>
       <c r="C32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B33" t="s">
         <v>10</v>
       </c>
       <c r="C33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B34" t="s">
         <v>11</v>
       </c>
+      <c r="C34" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B35" t="s">
         <v>8</v>
       </c>
       <c r="C35" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B36" t="s">
         <v>9</v>
       </c>
+      <c r="C36" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B37" t="s">
         <v>10</v>
       </c>
+      <c r="C37" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B38" t="s">
         <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B39" t="s">
         <v>8</v>
       </c>
-      <c r="C39" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B40" t="s">
         <v>9</v>
@@ -2897,7 +2779,7 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B41" t="s">
         <v>10</v>
@@ -2905,7 +2787,7 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B42" t="s">
         <v>11</v>
@@ -2913,18 +2795,15 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B43" t="s">
         <v>8</v>
       </c>
-      <c r="C43" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B44" t="s">
         <v>9</v>
@@ -2932,7 +2811,7 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B45" t="s">
         <v>10</v>
@@ -2940,51 +2819,39 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B46" t="s">
         <v>11</v>
       </c>
-      <c r="C46" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B47" t="s">
         <v>8</v>
       </c>
-      <c r="C47" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B48" t="s">
         <v>9</v>
       </c>
-      <c r="C48" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B49" t="s">
         <v>10</v>
       </c>
-      <c r="C49" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B50" t="s">
         <v>11</v>
@@ -2992,7 +2859,7 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B51" t="s">
         <v>8</v>
@@ -3003,86 +2870,92 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B52" t="s">
         <v>9</v>
       </c>
       <c r="C52" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B53" t="s">
         <v>10</v>
       </c>
       <c r="C53" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B54" t="s">
         <v>11</v>
       </c>
+      <c r="C54" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B55" t="s">
         <v>8</v>
       </c>
       <c r="C55" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B56" t="s">
         <v>9</v>
       </c>
+      <c r="C56" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B57" t="s">
         <v>10</v>
       </c>
+      <c r="C57" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B58" t="s">
         <v>11</v>
       </c>
       <c r="C58" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B59" t="s">
         <v>8</v>
       </c>
-      <c r="C59" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B60" t="s">
         <v>9</v>
@@ -3090,7 +2963,7 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B61" t="s">
         <v>10</v>
@@ -3098,7 +2971,7 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B62" t="s">
         <v>11</v>
@@ -3106,18 +2979,15 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B63" t="s">
         <v>8</v>
       </c>
-      <c r="C63" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B64" t="s">
         <v>9</v>
@@ -3125,7 +2995,7 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B65" t="s">
         <v>10</v>
@@ -3133,51 +3003,39 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B66" t="s">
         <v>11</v>
       </c>
-      <c r="C66" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B67" t="s">
         <v>8</v>
       </c>
-      <c r="C67" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B68" t="s">
         <v>9</v>
       </c>
-      <c r="C68" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B69" t="s">
         <v>10</v>
       </c>
-      <c r="C69" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B70" t="s">
         <v>11</v>
@@ -3185,7 +3043,7 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B71" t="s">
         <v>8</v>
@@ -3196,964 +3054,905 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B72" t="s">
         <v>9</v>
       </c>
       <c r="C72" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B73" t="s">
         <v>10</v>
       </c>
       <c r="C73" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B74" t="s">
         <v>11</v>
       </c>
+      <c r="C74" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B75" t="s">
         <v>8</v>
       </c>
       <c r="C75" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B76" t="s">
         <v>9</v>
       </c>
+      <c r="C76" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B77" t="s">
         <v>10</v>
       </c>
+      <c r="C77" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B78" t="s">
         <v>11</v>
       </c>
       <c r="C78" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B79" t="s">
         <v>8</v>
       </c>
-      <c r="C79" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B80" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B81" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B82" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B83" t="s">
         <v>8</v>
       </c>
-      <c r="C83" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3">
+    </row>
+    <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B84" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B85" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B86" t="s">
         <v>11</v>
       </c>
-      <c r="C86" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
+    </row>
+    <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B87" t="s">
         <v>8</v>
       </c>
-      <c r="C87" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
+    </row>
+    <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B88" t="s">
         <v>9</v>
       </c>
-      <c r="C88" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3">
+    </row>
+    <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B89" t="s">
         <v>10</v>
       </c>
-      <c r="C89" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
+    </row>
+    <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B90" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:2">
       <c r="A92" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
-      <c r="A93" s="12" t="s">
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
-      <c r="A94" t="s">
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3">
-      <c r="A95" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3">
-      <c r="A96" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="210" spans="1:1">
       <c r="A210" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="212" spans="1:1">
       <c r="A212" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="216" spans="1:1">
       <c r="A216" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="220" spans="1:1">
       <c r="A220" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="221" spans="1:1">
       <c r="A221" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="224" spans="1:1">
       <c r="A224" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="225" spans="1:1">
       <c r="A225" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="232" spans="1:1">
       <c r="A232" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="234" spans="1:1">
       <c r="A234" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="235" spans="1:1">
       <c r="A235" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="236" spans="1:1">
       <c r="A236" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="237" spans="1:1">
       <c r="A237" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="238" spans="1:1">
-      <c r="A238" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="239" spans="1:1">
-      <c r="A239" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="240" spans="1:1">
-      <c r="A240" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="241" spans="1:1">
-      <c r="A241" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="242" spans="1:1">
-      <c r="A242" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="243" spans="1:1">
-      <c r="A243" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="244" spans="1:1">
-      <c r="A244" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="245" spans="1:1">
-      <c r="A245" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="246" spans="1:1">
-      <c r="A246" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="247" spans="1:1">
-      <c r="A247" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>